<commit_message>
All FANN code. Much is not mine, this is a library developed by someone else
</commit_message>
<xml_diff>
--- a/32/specific exemplars_new.xlsx
+++ b/32/specific exemplars_new.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chrisweinberger/Documents/cogNeuroResearch/cogNeuro/32/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44176EBF-4FCD-D047-8A7F-C421488F697B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDC5DF64-9E86-7640-BB2E-E502727C8169}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2300" yWindow="640" windowWidth="21860" windowHeight="19540" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5320" yWindow="460" windowWidth="21860" windowHeight="19540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="specific exemplars_new" sheetId="1" r:id="rId1"/>
@@ -1073,8 +1073,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AI64"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="O42" sqref="O42"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="AJ6" sqref="AJ6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1287,6 +1287,10 @@
       <c r="AG2">
         <v>0</v>
       </c>
+      <c r="AI2">
+        <f>CORREL(B2:AG2,B3:AG3)</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="3" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
@@ -1389,7 +1393,7 @@
         <v>0</v>
       </c>
       <c r="AI3">
-        <f t="shared" ref="AI3" si="0">CORREL(B3:AG3,B4:AG4)</f>
+        <f>CORREL(B3:AG3,B4:AG4)</f>
         <v>0.75</v>
       </c>
     </row>
@@ -1493,6 +1497,10 @@
       <c r="AG4">
         <v>0</v>
       </c>
+      <c r="AI4">
+        <f>CORREL(B4:AG4,B5:AG5)</f>
+        <v>-0.25</v>
+      </c>
     </row>
     <row r="5" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
@@ -1595,7 +1603,7 @@
         <v>1</v>
       </c>
       <c r="AI5">
-        <f t="shared" ref="AI5" si="1">CORREL(B5:AG5,B6:AG6)</f>
+        <f t="shared" ref="AI5:AI62" si="0">CORREL(B5:AG5,B6:AG6)</f>
         <v>0.75</v>
       </c>
     </row>
@@ -1699,6 +1707,10 @@
       <c r="AG6">
         <v>1</v>
       </c>
+      <c r="AI6">
+        <f t="shared" si="0"/>
+        <v>-0.125</v>
+      </c>
     </row>
     <row r="7" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
@@ -1801,7 +1813,7 @@
         <v>0</v>
       </c>
       <c r="AI7">
-        <f t="shared" ref="AI7" si="2">CORREL(B7:AG7,B8:AG8)</f>
+        <f t="shared" si="0"/>
         <v>0.75</v>
       </c>
     </row>
@@ -1905,6 +1917,10 @@
       <c r="AG8">
         <v>0</v>
       </c>
+      <c r="AI8">
+        <f t="shared" si="0"/>
+        <v>-0.125</v>
+      </c>
     </row>
     <row r="9" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
@@ -2007,7 +2023,7 @@
         <v>1</v>
       </c>
       <c r="AI9">
-        <f t="shared" ref="AI9" si="3">CORREL(B9:AG9,B10:AG10)</f>
+        <f t="shared" si="0"/>
         <v>0.75</v>
       </c>
     </row>
@@ -2111,6 +2127,10 @@
       <c r="AG10">
         <v>1</v>
       </c>
+      <c r="AI10">
+        <f t="shared" si="0"/>
+        <v>-0.125</v>
+      </c>
     </row>
     <row r="11" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
@@ -2213,7 +2233,7 @@
         <v>1</v>
       </c>
       <c r="AI11">
-        <f t="shared" ref="AI11" si="4">CORREL(B11:AG11,B12:AG12)</f>
+        <f t="shared" si="0"/>
         <v>0.75</v>
       </c>
     </row>
@@ -2317,6 +2337,10 @@
       <c r="AG12">
         <v>1</v>
       </c>
+      <c r="AI12">
+        <f t="shared" si="0"/>
+        <v>0.125</v>
+      </c>
     </row>
     <row r="13" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
@@ -2419,7 +2443,7 @@
         <v>0</v>
       </c>
       <c r="AI13">
-        <f t="shared" ref="AI13" si="5">CORREL(B13:AG13,B14:AG14)</f>
+        <f t="shared" si="0"/>
         <v>0.75</v>
       </c>
     </row>
@@ -2523,6 +2547,10 @@
       <c r="AG14">
         <v>0</v>
       </c>
+      <c r="AI14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="15" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
@@ -2625,7 +2653,7 @@
         <v>0</v>
       </c>
       <c r="AI15">
-        <f t="shared" ref="AI15" si="6">CORREL(B15:AG15,B16:AG16)</f>
+        <f t="shared" si="0"/>
         <v>0.75</v>
       </c>
     </row>
@@ -2729,6 +2757,10 @@
       <c r="AG16">
         <v>0</v>
       </c>
+      <c r="AI16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="17" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
@@ -2831,7 +2863,7 @@
         <v>1</v>
       </c>
       <c r="AI17">
-        <f t="shared" ref="AI17" si="7">CORREL(B17:AG17,B18:AG18)</f>
+        <f t="shared" si="0"/>
         <v>0.75</v>
       </c>
     </row>
@@ -2935,6 +2967,10 @@
       <c r="AG18">
         <v>1</v>
       </c>
+      <c r="AI18">
+        <f t="shared" si="0"/>
+        <v>0.125</v>
+      </c>
     </row>
     <row r="19" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
@@ -3037,7 +3073,7 @@
         <v>1</v>
       </c>
       <c r="AI19">
-        <f t="shared" ref="AI19" si="8">CORREL(B19:AG19,B20:AG20)</f>
+        <f t="shared" si="0"/>
         <v>0.75</v>
       </c>
     </row>
@@ -3141,6 +3177,10 @@
       <c r="AG20">
         <v>1</v>
       </c>
+      <c r="AI20">
+        <f t="shared" si="0"/>
+        <v>-0.125</v>
+      </c>
     </row>
     <row r="21" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
@@ -3243,7 +3283,7 @@
         <v>1</v>
       </c>
       <c r="AI21">
-        <f t="shared" ref="AI21" si="9">CORREL(B21:AG21,B22:AG22)</f>
+        <f t="shared" si="0"/>
         <v>0.75</v>
       </c>
     </row>
@@ -3347,6 +3387,10 @@
       <c r="AG22">
         <v>0</v>
       </c>
+      <c r="AI22">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="23" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
@@ -3449,7 +3493,7 @@
         <v>1</v>
       </c>
       <c r="AI23">
-        <f t="shared" ref="AI23" si="10">CORREL(B23:AG23,B24:AG24)</f>
+        <f t="shared" si="0"/>
         <v>0.75</v>
       </c>
     </row>
@@ -3553,6 +3597,10 @@
       <c r="AG24">
         <v>1</v>
       </c>
+      <c r="AI24">
+        <f t="shared" si="0"/>
+        <v>-0.125</v>
+      </c>
     </row>
     <row r="25" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
@@ -3655,7 +3703,7 @@
         <v>0</v>
       </c>
       <c r="AI25">
-        <f t="shared" ref="AI25" si="11">CORREL(B25:AG25,B26:AG26)</f>
+        <f t="shared" si="0"/>
         <v>0.75</v>
       </c>
     </row>
@@ -3759,6 +3807,10 @@
       <c r="AG26">
         <v>0</v>
       </c>
+      <c r="AI26">
+        <f t="shared" si="0"/>
+        <v>-0.125</v>
+      </c>
     </row>
     <row r="27" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
@@ -3861,7 +3913,7 @@
         <v>0</v>
       </c>
       <c r="AI27">
-        <f t="shared" ref="AI27" si="12">CORREL(B27:AG27,B28:AG28)</f>
+        <f t="shared" si="0"/>
         <v>0.75</v>
       </c>
     </row>
@@ -3965,6 +4017,10 @@
       <c r="AG28">
         <v>0</v>
       </c>
+      <c r="AI28">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="29" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
@@ -4067,7 +4123,7 @@
         <v>1</v>
       </c>
       <c r="AI29">
-        <f t="shared" ref="AI29" si="13">CORREL(B29:AG29,B30:AG30)</f>
+        <f t="shared" si="0"/>
         <v>0.75</v>
       </c>
     </row>
@@ -4171,6 +4227,10 @@
       <c r="AG30">
         <v>1</v>
       </c>
+      <c r="AI30">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="31" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
@@ -4273,7 +4333,7 @@
         <v>0</v>
       </c>
       <c r="AI31">
-        <f t="shared" ref="AI31" si="14">CORREL(B31:AG31,B32:AG32)</f>
+        <f t="shared" si="0"/>
         <v>0.75</v>
       </c>
     </row>
@@ -4377,6 +4437,10 @@
       <c r="AG32">
         <v>0</v>
       </c>
+      <c r="AI32">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="33" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
@@ -4479,7 +4543,7 @@
         <v>1</v>
       </c>
       <c r="AI33">
-        <f t="shared" ref="AI33" si="15">CORREL(B33:AG33,B34:AG34)</f>
+        <f t="shared" si="0"/>
         <v>0.75</v>
       </c>
     </row>
@@ -4583,6 +4647,10 @@
       <c r="AG34">
         <v>1</v>
       </c>
+      <c r="AI34">
+        <f t="shared" si="0"/>
+        <v>-0.125</v>
+      </c>
     </row>
     <row r="35" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
@@ -4685,7 +4753,7 @@
         <v>1</v>
       </c>
       <c r="AI35">
-        <f t="shared" ref="AI35" si="16">CORREL(B35:AG35,B36:AG36)</f>
+        <f t="shared" si="0"/>
         <v>0.75</v>
       </c>
     </row>
@@ -4789,6 +4857,10 @@
       <c r="AG36">
         <v>1</v>
       </c>
+      <c r="AI36">
+        <f t="shared" si="0"/>
+        <v>0.125</v>
+      </c>
     </row>
     <row r="37" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
@@ -4891,7 +4963,7 @@
         <v>0</v>
       </c>
       <c r="AI37">
-        <f t="shared" ref="AI37" si="17">CORREL(B37:AG37,B38:AG38)</f>
+        <f t="shared" si="0"/>
         <v>0.75</v>
       </c>
     </row>
@@ -4995,6 +5067,10 @@
       <c r="AG38">
         <v>0</v>
       </c>
+      <c r="AI38">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="39" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
@@ -5097,7 +5173,7 @@
         <v>1</v>
       </c>
       <c r="AI39">
-        <f t="shared" ref="AI39" si="18">CORREL(B39:AG39,B40:AG40)</f>
+        <f t="shared" si="0"/>
         <v>0.75</v>
       </c>
     </row>
@@ -5201,6 +5277,10 @@
       <c r="AG40">
         <v>1</v>
       </c>
+      <c r="AI40">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="41" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
@@ -5303,7 +5383,7 @@
         <v>0</v>
       </c>
       <c r="AI41">
-        <f t="shared" ref="AI41" si="19">CORREL(B41:AG41,B42:AG42)</f>
+        <f t="shared" si="0"/>
         <v>0.75</v>
       </c>
     </row>
@@ -5407,6 +5487,10 @@
       <c r="AG42">
         <v>0</v>
       </c>
+      <c r="AI42">
+        <f t="shared" si="0"/>
+        <v>-0.125</v>
+      </c>
     </row>
     <row r="43" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
@@ -5509,7 +5593,7 @@
         <v>0</v>
       </c>
       <c r="AI43">
-        <f t="shared" ref="AI43" si="20">CORREL(B43:AG43,B44:AG44)</f>
+        <f t="shared" si="0"/>
         <v>0.75</v>
       </c>
     </row>
@@ -5613,6 +5697,10 @@
       <c r="AG44">
         <v>0</v>
       </c>
+      <c r="AI44">
+        <f t="shared" si="0"/>
+        <v>0.125</v>
+      </c>
     </row>
     <row r="45" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
@@ -5715,7 +5803,7 @@
         <v>1</v>
       </c>
       <c r="AI45">
-        <f t="shared" ref="AI45" si="21">CORREL(B45:AG45,B46:AG46)</f>
+        <f t="shared" si="0"/>
         <v>0.75</v>
       </c>
     </row>
@@ -5819,6 +5907,10 @@
       <c r="AG46">
         <v>1</v>
       </c>
+      <c r="AI46">
+        <f t="shared" si="0"/>
+        <v>-0.25</v>
+      </c>
     </row>
     <row r="47" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
@@ -5921,7 +6013,7 @@
         <v>1</v>
       </c>
       <c r="AI47">
-        <f t="shared" ref="AI47" si="22">CORREL(B47:AG47,B48:AG48)</f>
+        <f t="shared" si="0"/>
         <v>0.75</v>
       </c>
     </row>
@@ -6025,6 +6117,10 @@
       <c r="AG48">
         <v>1</v>
       </c>
+      <c r="AI48">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="49" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
@@ -6127,7 +6223,7 @@
         <v>0</v>
       </c>
       <c r="AI49">
-        <f t="shared" ref="AI49" si="23">CORREL(B49:AG49,B50:AG50)</f>
+        <f t="shared" si="0"/>
         <v>0.75</v>
       </c>
     </row>
@@ -6231,6 +6327,10 @@
       <c r="AG50">
         <v>0</v>
       </c>
+      <c r="AI50">
+        <f t="shared" si="0"/>
+        <v>0.125</v>
+      </c>
     </row>
     <row r="51" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
@@ -6333,7 +6433,7 @@
         <v>0</v>
       </c>
       <c r="AI51">
-        <f t="shared" ref="AI51" si="24">CORREL(B51:AG51,B52:AG52)</f>
+        <f t="shared" si="0"/>
         <v>0.75</v>
       </c>
     </row>
@@ -6437,6 +6537,10 @@
       <c r="AG52">
         <v>0</v>
       </c>
+      <c r="AI52">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="53" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
@@ -6539,7 +6643,7 @@
         <v>1</v>
       </c>
       <c r="AI53">
-        <f t="shared" ref="AI53" si="25">CORREL(B53:AG53,B54:AG54)</f>
+        <f t="shared" si="0"/>
         <v>0.75</v>
       </c>
     </row>
@@ -6643,6 +6747,10 @@
       <c r="AG54">
         <v>1</v>
       </c>
+      <c r="AI54">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="55" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
@@ -6745,7 +6853,7 @@
         <v>0</v>
       </c>
       <c r="AI55">
-        <f t="shared" ref="AI55" si="26">CORREL(B55:AG55,B56:AG56)</f>
+        <f t="shared" si="0"/>
         <v>0.75</v>
       </c>
     </row>
@@ -6849,6 +6957,10 @@
       <c r="AG56">
         <v>0</v>
       </c>
+      <c r="AI56">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="57" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
@@ -6951,7 +7063,7 @@
         <v>1</v>
       </c>
       <c r="AI57">
-        <f t="shared" ref="AI57" si="27">CORREL(B57:AG57,B58:AG58)</f>
+        <f t="shared" si="0"/>
         <v>0.75</v>
       </c>
     </row>
@@ -7055,6 +7167,10 @@
       <c r="AG58">
         <v>1</v>
       </c>
+      <c r="AI58">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="59" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
@@ -7157,7 +7273,7 @@
         <v>1</v>
       </c>
       <c r="AI59">
-        <f t="shared" ref="AI59" si="28">CORREL(B59:AG59,B60:AG60)</f>
+        <f t="shared" si="0"/>
         <v>0.75</v>
       </c>
     </row>
@@ -7261,6 +7377,10 @@
       <c r="AG60">
         <v>1</v>
       </c>
+      <c r="AI60">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="61" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
@@ -7363,7 +7483,7 @@
         <v>0</v>
       </c>
       <c r="AI61">
-        <f t="shared" ref="AI61" si="29">CORREL(B61:AG61,B62:AG62)</f>
+        <f t="shared" si="0"/>
         <v>0.75</v>
       </c>
     </row>
@@ -7467,6 +7587,10 @@
       <c r="AG62">
         <v>0</v>
       </c>
+      <c r="AI62">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="63" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
@@ -7569,7 +7693,7 @@
         <v>1</v>
       </c>
       <c r="AI63">
-        <f t="shared" ref="AI63" si="30">CORREL(B63:AG63,B64:AG64)</f>
+        <f t="shared" ref="AI63" si="1">CORREL(B63:AG63,B64:AG64)</f>
         <v>-6.6666666666666652E-2</v>
       </c>
     </row>
@@ -7683,8 +7807,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3119604E-45F9-F843-A903-89D0570F901C}">
   <dimension ref="A1:AI32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="AT14" sqref="AT14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H37" sqref="H37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>